<commit_message>
modified input template and simplified serviceTypeCodes / PracticeTypeCode interactions
</commit_message>
<xml_diff>
--- a/templates/test_patients.xlsx
+++ b/templates/test_patients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/craig.gifford/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/craig.gifford/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1112DAAE-A0FB-6344-8B67-9660C299FEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA9D6FC7-6ACF-5948-976F-FECF0B210437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34080" yWindow="4300" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="2980" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="On" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Customer</t>
   </si>
@@ -42,6 +42,12 @@
     <t>Type</t>
   </si>
   <si>
+    <t>Payer ID Stedi</t>
+  </si>
+  <si>
+    <t>Payer ID pVerify</t>
+  </si>
+  <si>
     <t>Payer Name</t>
   </si>
   <si>
@@ -66,35 +72,17 @@
     <t>Subscriber DOB</t>
   </si>
   <si>
-    <t>isSubPat</t>
-  </si>
-  <si>
-    <t>Patient First</t>
-  </si>
-  <si>
-    <t>Patient Last</t>
-  </si>
-  <si>
-    <t>Patient DOB</t>
-  </si>
-  <si>
-    <t>Working</t>
-  </si>
-  <si>
-    <t>PATLINK</t>
-  </si>
-  <si>
-    <t>Payer ID Stedi</t>
-  </si>
-  <si>
-    <t>Payer ID pVerify</t>
+    <t>Stedi Service Code</t>
+  </si>
+  <si>
+    <t>pVerify Service Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,7 +92,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -112,6 +100,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -142,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,18 +147,24 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,140 +473,128 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="5" customWidth="1"/>
-    <col min="2" max="3" width="20" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36" style="5" customWidth="1"/>
-    <col min="6" max="6" width="36.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="12.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" style="10" customWidth="1"/>
+    <col min="8" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -618,82 +606,72 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.83203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>